<commit_message>
null check daale-initialQuizeData, dataa hataayaa dono excel se
</commit_message>
<xml_diff>
--- a/Question-file.xlsx
+++ b/Question-file.xlsx
@@ -1,46 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Sheet2" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="Sheet3" state="visible" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>user</t>
+    <t>index</t>
   </si>
   <si>
-    <t>result</t>
-  </si>
-  <si>
-    <t>{"quiz_questions":[{"id":"1","question":"Sparing in words, using very few words","possible_answers":"Loquacious,Laconic,Integral,Judicious","correct_answer":"2"},{"id":"2","question":"Freedom from punishment","possible_answers":"Impunity,Indolent,Jaded,Hedonist","correct_answer":"1"},{"id":"3","question":"An instrument for measuring","possible_answers":"Gallant ,Gauge ,Gamester ,Gastric ","correct_answer":"2"},{"id":"4","question":"Inflammation of the stomach  ","possible_answers":"Insurgent ,Impudence ,Garrulous ,Gastritis ","correct_answer":"4"},{"id”:”5”,”question":"unoriginal","possible_answers":"Imperious ,Impudence ,Hackneyed ,Inane ","correct_answer":"3"},{"id”:”6”,”question":"To draw principle inferences","possible_answers":"Gaseous ,Generalize ,Garrote ,Garrison ","correct_answer":"2"},{"id”:”7”,”question":"To imbue with life or animation ","possible_answers":"Galvanize ,Garnish ,Garrulous ,Gaseous ","correct_answer":"1"},{"id”:”8”,”question":"Decorate or embellish ","possible_answers":"Gamut ,Genealogist ,Gambol ,Garnish ","correct_answer":"4"},{"id”:”9”,”question":"Given to constant trivial talking","possible_answers":"Gaseous ,Gendarme ,Garrulous ,Genitive ","correct_answer":"3"},{"id”:”10”,”question":"To risk money or other possession on an event","possible_answers":"Gallant ,Gaily ,Gamble ,Gastronomy ","correct_answer":"3"},{"id”:”11”,”question":"A tracer of pedigrees","possible_answers":"Genealogist ,Genealogy ,Generic ,Gentile ","correct_answer":"1"},{"id":"12","question":"Loud and flashy","possible_answers":"Garish ,Indolent,Jaded,Hedonist","correct_answer":"1"},{"id":"13","question":"anything that foreshadows the future event","possible_answers":"Hedonist ,Harbinger ,Implicit ,Inane ","correct_answer":"2"},{"id":"14","question":"a person’s manner of walking","possible_answers":"Gaily ,Gait ,Gauge ,Galvanize ","correct_answer":"2"},{"id”:”15”,”question":"A whole range or sequence","possible_answers":"Garrulous ,Indolent,Gambol ,Gamut ","correct_answer":"4"},{"id”:”16”,”question":"To produce or cause to be","possible_answers":"Generate ,Generosity ,Harbinger, Gendarme","correct_answer":"1"},{"id":"17","question":"Easily persuaded to believe something ","possible_answers":"Glutton , Jaded,Gregarious ,Gullible ","correct_answer":"4"},{"id":"18","question":"The quality of being kind and generous","possible_answers":"Genesis , Generosity, Gallant, Garrote","correct_answer":"2"},{"id":"19","question":"Festivity, the state of being lighthearted or cheerful","possible_answers":"Gait ,Gaiety ,Gallant ,Gamester ","correct_answer":"2"},{"id":"20","question":"Abundant","possible_answers":"Galore ,Garrison ,Gamble ,Gendarme ","correct_answer":"1"},{"id":"21","question":"Light and unsubstantial","possible_answers":"Gastritis ,Garrison ,Gaseous ,Genealogy ","correct_answer":"3"},{"id":"22","question":"refined or respectable","possible_answers":"Impunity,Genitive ,Genteel ,Garish ","correct_answer":"3"},{"id":"23","question":"habitual overeater","possible_answers":"Gregarious ,Glutton ,Grandiose ,Gullible ","correct_answer":"2"},{"id":"24","question":"A person who pursue pleasure, often to excess","possible_answers":"Impunity,Indolent,Jaded,Hedonist","correct_answer":"4"},{"id":"25","question":"Exaggeration","possible_answers":"Hyperbole ,Indolent,Impudence ,Impeccable ","correct_answer":"1"},{"id":"26","question":"Arrogant","possible_answers":"Loquacious,Laconic,Imperious ,Implicit ","correct_answer":"3"},{"id":"27","question":"Stupid, pointless, absurd","possible_answers":"Inane ,Indolent,Jaded,Hedonist","correct_answer":"1"},{"id":"28","question":"Poor, needy","possible_answers":"Gallant ,Indigent  ,Insipid  ,Indolent  ","correct_answer":"2"},{"id":"29","question":"notorious","possible_answers":"Insurgent ,Impudence ,Garrulous ,Infamous  ","correct_answer":"4"},{"id":"30","question":"Dull, boring, lifeless","possible_answers":"Imperious ,Impudence ,Insipid  ,Inane ","correct_answer":"3"},{"id":"31","question":"Rebellious","possible_answers":"Gaseous ,Insurgent  ,Garrote ,Integral  ","correct_answer":"2"},{"id”:”32”,”question":"Looking inward ","possible_answers":"Introspective  , Indigent , Imperious , Laconic ","correct_answer":"1"},{"id":"33","question":"Faultless, perfect ","possible_answers":"Gamut , Indolent ,Imperious  ,Impeccable  ","correct_answer":"4"},{"id":"34","question":"Essential, necessary","possible_answers":"Laconic  ,Jaded  ,Integral  ,Genitive ","correct_answer":"3"},{"id":"35","question":"Talkative","possible_answers":"Gallant , Laconic ,Loquacious  ,Listless  ","correct_answer":"3"},{"id”:”36”,”question":"wise, marked by good judgment","possible_answers":"Judicious   , Insurgent , Indigent ,Gentile ","correct_answer":"1"},{"id”:”37”,”question":"Good natured, merry, given to joking, cheerful and friendly","possible_answers":"Jovial  ,Indolent,Kinetic ,Laud ","correct_answer":"1"},{"id":"38","question":"Impressive or magnificent in appearance or style, excessively grand or ambitious","possible_answers":"Hedonist ,Grandiose  ,Implicit ,Inane ","correct_answer":"2"},{"id":"39","question":"of pertaining to, or near the stomach","possible_answers":"Gaily ,Gastric  ,Gauge ,Gait ","correct_answer":"2"},{"id":"40","question":" A list, in the order of succession, of ancestors and their descendants","possible_answers":"Garrulous ,Generality ,Gambol ,Genealogy  ","correct_answer":"4"},{"id”:”41”,”question":"In a cheerful or lighthearted way, without thinking of consequences, Merrily","possible_answers":"Gaily  ,Generosity ,Harbinger, Gullible","correct_answer":"1"},{"id":"42","question":"To execute by strangling","possible_answers":"Glutton , Jaded,Gregarious ,Garrote  ","correct_answer":"4"},{"id":"43","question":"habitual overeater","possible_answers":"Genesis , Glutton , Gallant, Garrote","correct_answer":"2"},{"id":"44","question":"Stupid, pointless, absurd","possible_answers":"Gait ,Inane  , Insipid , Indolent ","correct_answer":"2"},{"id":"45","question":"Pertaining to motion","possible_answers":"Galore ,Kinetic  , Garrulous ,Gendarme ","correct_answer":"2"},{"id":"46","question":"Lazy","possible_answers":"Innate  ,Infamous  ,Indolent  ,Indigent  ","correct_answer":"3"},{"id":"47","question":"Sparing in words, using very few words","possible_answers":"Impunity,Genitive ,Laconic  ,Garish ","correct_answer":"3"},{"id":"48","question":"habitual overeater","possible_answers":"Gregarious ,Glutton ,Grandiose ,Gullible ","correct_answer":"2"},{"id":"49","question":"Tired, bored, or lacking enthusiasm, typically after having too much of something","possible_answers":"Impunity,Indolent, Grandiose, Jaded","correct_answer":"4"},{"id”:”50”,”question":"Talkative","possible_answers":"Loquacious  ,Laconic ,Impudence ,Jaded  ","correct_answer":"1"}]}</t>
-  </si>
-  <si>
-    <t>{"quiz_questions":[{"id":"1","question":"Sparing in words, using very few words","possible_answers":"Loquacious,Laconic,Integral,Judicious","correct_answer":"2"},{"id":"2","question":"Freedom from punishment","possible_answers":"Impunity,Indolent,Jaded,Hedonist","correct_answer":"1"},{"id":"3","question":"An instrument for measuring","possible_answers":"Gallant ,Gauge ,Gamester ,Gastric ","correct_answer":"2"},{"id":"4","question":"Inflammation of the stomach  ","possible_answers":"Insurgent ,Impudence ,Garrulous ,Gastritis ","correct_answer":"4"},{"id”:”5”,”question":"unoriginal","possible_answers":"Imperious ,Impudence ,Hackneyed ,Inane ","correct_answer":"3"},{"id”:”6”,”question":"To draw principle inferences","possible_answers":"Gaseous ,Generalize ,Garrote ,Garrison ","correct_answer":"2"},{"id”:”7”,”question":"To imbue with life or animation ","possible_answers":"Galvanize ,Garnish ,Garrulous ,Gaseous ","correct_answer":"1"},{"id”:”8”,”question":"Decorate or embellish ","possible_answers":"Gamut ,Genealogist ,Gambol ,Garnish ","correct_answer":"4"},{"id”:”9”,”question":"Given to constant trivial talking","possible_answers":"Gaseous ,Gendarme ,Garrulous ,Genitive ","correct_answer":"3"},{"id”:”10”,”question":"To risk money or other possession on an event","possible_answers":"Gallant ,Gaily ,Gamble ,Gastronomy ","correct_answer":"3"}]}</t>
+    <t>json</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -70,13 +64,10 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -369,15 +360,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -385,38 +376,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -424,11 +383,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -436,11 +395,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
khaali datat intialQuize me hal kar diyaa shrimaan
</commit_message>
<xml_diff>
--- a/Question-file.xlsx
+++ b/Question-file.xlsx
@@ -1,40 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Sheet2" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="Sheet3" state="visible" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>index</t>
   </si>
   <si>
     <t>json</t>
   </si>
+  <si>
+    <t>{"quiz_questions":[{"id":"1","question":"Sparing in words, using very few words","possible_answers":"Loquacious,Laconic,Integral,Judicious","correct_answer":"2"},{"id":"2","question":"Freedom from punishment","possible_answers":"Impunity,Indolent,Jaded,Hedonist","correct_answer":"1"},{"id":"3","question":"An instrument for measuring","possible_answers":"Gallant ,Gauge ,Gamester ,Gastric ","correct_answer":"2"},{"id":"4","question":"Inflammation of the stomach  ","possible_answers":"Insurgent ,Impudence ,Garrulous ,Gastritis ","correct_answer":"4"},{"id”:”5”,”question":"unoriginal","possible_answers":"Imperious ,Impudence ,Hackneyed ,Inane ","correct_answer":"3"},{"id”:”6”,”question":"To draw principle inferences","possible_answers":"Gaseous ,Generalize ,Garrote ,Garrison ","correct_answer":"2"},{"id”:”7”,”question":"To imbue with life or animation ","possible_answers":"Galvanize ,Garnish ,Garrulous ,Gaseous ","correct_answer":"1"},{"id”:”8”,”question":"Decorate or embellish ","possible_answers":"Gamut ,Genealogist ,Gambol ,Garnish ","correct_answer":"4"},{"id”:”9”,”question":"Given to constant trivial talking","possible_answers":"Gaseous ,Gendarme ,Garrulous ,Genitive ","correct_answer":"3"},{"id”:”10”,”question":"To risk money or other possession on an event","possible_answers":"Gallant ,Gaily ,Gamble ,Gastronomy ","correct_answer":"3"}]}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -64,10 +67,13 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -360,20 +366,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -383,11 +413,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -395,11 +425,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
prashna badal diye hai
</commit_message>
<xml_diff>
--- a/Question-file.xlsx
+++ b/Question-file.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Sheet2" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="Sheet3" state="visible" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>index</t>
   </si>
@@ -24,20 +24,20 @@
     <t>json</t>
   </si>
   <si>
-    <t>{"quiz_questions":[{"id":"1","question":"Sparing in words, using very few words","possible_answers":"Loquacious,Laconic,Integral,Judicious","correct_answer":"2"},{"id":"2","question":"Freedom from punishment","possible_answers":"Impunity,Indolent,Jaded,Hedonist","correct_answer":"1"},{"id":"3","question":"An instrument for measuring","possible_answers":"Gallant ,Gauge ,Gamester ,Gastric ","correct_answer":"2"},{"id":"4","question":"Inflammation of the stomach  ","possible_answers":"Insurgent ,Impudence ,Garrulous ,Gastritis ","correct_answer":"4"},{"id”:”5”,”question":"unoriginal","possible_answers":"Imperious ,Impudence ,Hackneyed ,Inane ","correct_answer":"3"},{"id”:”6”,”question":"To draw principle inferences","possible_answers":"Gaseous ,Generalize ,Garrote ,Garrison ","correct_answer":"2"},{"id”:”7”,”question":"To imbue with life or animation ","possible_answers":"Galvanize ,Garnish ,Garrulous ,Gaseous ","correct_answer":"1"},{"id”:”8”,”question":"Decorate or embellish ","possible_answers":"Gamut ,Genealogist ,Gambol ,Garnish ","correct_answer":"4"},{"id”:”9”,”question":"Given to constant trivial talking","possible_answers":"Gaseous ,Gendarme ,Garrulous ,Genitive ","correct_answer":"3"},{"id”:”10”,”question":"To risk money or other possession on an event","possible_answers":"Gallant ,Gaily ,Gamble ,Gastronomy ","correct_answer":"3"}]}</t>
+    <t>{"quiz_questions":[{"id":"1","question":"Name\nAnnie\nBob\nCallie\nDerek\n\nWhich of these query will display the the table given above ?\n","possible_answers":"Select employee from name,Select name,Select name from employee,Select employee","correct_answer":"3"},{"id":"2","question":"Here which of the following displays the unique values of the column?\n\n   SELECT ________ dept_name \n   FROM instructor;\n","possible_answers":"All,From,Distinct,Name","correct_answer":"3"},{"id":"3","question":"This Query can be replaced by which one of the following?\n\n   SELECT name, course_id\n   FROM instructor, teaches\n   WHERE instructor_ID= teaches_ID;\n","possible_answers":"Select name,course_id from teaches,instructor where instructor_id=course_id;,Select name, course_id from instructor natural join teaches;,Select name, course_id from instructor; ,Select course_id from instructor join teaches;","correct_answer":"2"},{"id":"4","question":"SELECT * FROM employee WHERE salary&gt;10000 AND dept_id=101;\nWhich of the following fields are displayed as output?\n","possible_answers":"Salary, dept_id ,Employee ,Salary,All the field of employee relation","correct_answer":"4"},{"id":"5","question":"Which of the following statements contains an error?","possible_answers":"Select * from emp where empid = 10003; ,Select empid from emp where empid = 10006; ,Select empid from emp; ,Select empid where empid = 1009 and lastname = ‘GELLER’;","correct_answer":"4"},{"id":"6","question":"In the given query which of the keyword has to be inserted?\n\nINSERT INTO employee _____ (1002,Joey,2000);\n","possible_answers":"Table ,Values ,Relation ,Field ","correct_answer":"2"} ,{"id":"7","question":"Which of the following makes the transaction permanent in the database? ","possible_answers":"View ,Commit ,Rollback ,Flashback ","correct_answer":"2"} ,{"id":"8","question":"In order to undo the work of transaction after last commit which one should be used? ","possible_answers":"View ,Commit ,Rollback ,Flashback ","correct_answer":"3"} ,{"id":"9","question":"To include integrity constraint in an existing relation use :","possible_answers":"Create table ,Modify table ,Alter table ,Drop table ","correct_answer":"3"} ,{"id":"10","question":"Which of the following statements creates a new table temp instructor that has the same schema as an instructor.","possible_answers":"create table temp_instructor; ,create table temp_instructor like instructor; ,create Table as temp_instructor; ,create table like temp_instructor; ","correct_answer":"2"} ,{"id":"11","question":"Foreign key is the one in which the ________ of one relation is referenced in another relation.","possible_answers":"Foreign key ,Primary key ,References ,Check constraint ","correct_answer":"2"} ,{"id":"12","question":"SELECT emp_name\nFROM department\nWHERE dept_name LIKE ’ _____ Computer Science’;\nWhich one of the following has to be added into the blank to select the dept_name which has Computer Science as its ending string?\n","possible_answers":"% ,_ ,|| ,$ ","correct_answer":"1"} ,{"id":"13","question":"The term attribute refers to a ___________ of a table.","possible_answers":"Record ,Column ,Tuple ,Key ","correct_answer":"2"} ,{"id":"14","question":"For each attribute of a relation, there is a set of permitted values, called the ________ of that attribute.","possible_answers":"Domain ,Relation ,Set ,Schema ","correct_answer":"1"} ,{"id":"15","question":"Dates must be specified in the format","possible_answers":"mm/dd/yy ,yyyy/mm/dd ,dd/mm/yy ,yy/dd/mm ","correct_answer":"2"} ,{"id":"16","question":"CREATE DOMAIN YearlySalary NUMERIC(8,2)\nCONSTRAINT salary VALUE test __________;\nIn order to ensure that an instructor’s salary domain allows only values greater than a specified value use:\n","possible_answers":"Value&gt;=30000.00 ,Not null; ,Check(value &gt;= 29000.00); ,Check(value) ","correct_answer":"3"} ,{"id":"17","question":"Course(course_id,sec_id,semester)\nHere the course_id,sec_id and semester are __________ and course is a _________\n","possible_answers":"Relations/Attribute ,Attributes/Relation ,Tuple/Relation ,Tuple/Attributes ","correct_answer":"2"} ,{"id":"18","question":"SELECT name\nFROM instructor\nWHERE salary IS NOT NULL;\nSelects\n","possible_answers":"Tuples with null value ,Tuples with no null values ,Tuples with any salary ,All of the mentioned ","correct_answer":"2"} ,{"id":"19","question":"In an employee table to include the attributes whose value always have some value which of the following constraint must be used?","possible_answers":"Null ,Not null ,Unique ,Distinct ","correct_answer":"2"} ,{"id":"20","question":"Which one of the following is used to define the structure of the relation, deleting relations and relating schemas?","possible_answers":"DML(Data Manipulation Langauge) ,DDL(Data Definition Langauge) ,Query ,Relational Schema ","correct_answer":"2"} ,{"id":"21","question":"The primary key must be","possible_answers":"Unique ,Not null ,Both Unique and Not null ,Either Unique or Not null ","correct_answer":"3"} ,{"id":"22","question":"How many tables may be included with a join?","possible_answers":"One ,Two ,Three ,All of the mentioned ","correct_answer":"4"} ,{"id":"23","question":"Which one of the following attribute can be taken as a primary key?","possible_answers":"Name ,Street ,Id ,Department ","correct_answer":"3"} ,{"id":"24","question":"The default extension for an Oracle SQL*Plus file is:","possible_answers":".txt ,.pls ,.ora ,.sql ","correct_answer":"4"} ,{"id":"25","question":"Which of the following deletes all tuples in the instructor relation for those instructors associated with a department located in the Watson building which is in department relation.","possible_answers":"DELETE FROM instructor\n   WHERE dept_name IN 'Watson';\n ,DELETE FROM department \n   WHERE building='Watson';\n ,DELETE FROM instructor\nWHERE dept_name IN (SELECT dept name\nFROM department\nWHERE building = ’Watson’);\n ,None of the mentioned ","correct_answer":"3"} ]}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -67,13 +67,10 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -366,15 +363,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -382,7 +379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -390,22 +387,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -413,11 +394,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -425,11 +406,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>